<commit_message>
SSDM-13163 Adding support for warnings.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB30E29D-5B36-674A-95F7-BA1FDA634FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88B73ED-8155-594C-BD6E-AF1323B7195B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="36920" windowHeight="17500" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Code</t>
   </si>
@@ -77,9 +77,6 @@
     <t>STORAGES_COLLECTION</t>
   </si>
   <si>
-    <t>Storages Collection</t>
-  </si>
-  <si>
     <t>EXPERIMENTAL_STEP</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
   </si>
   <si>
     <t>TEST</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
   <si>
     <t>DEFAULT_SAMPLE</t>
@@ -151,12 +145,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -184,12 +183,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -501,7 +506,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,28 +566,24 @@
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -600,7 +601,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -619,12 +620,12 @@
         <v>10</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>4</v>

</xml_diff>